<commit_message>
finished enpoints for generating files
</commit_message>
<xml_diff>
--- a/src/static/reports/InfoCarreras.xlsx
+++ b/src/static/reports/InfoCarreras.xlsx
@@ -450,13 +450,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -466,13 +466,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -482,10 +482,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
fixed a problem with the create cathedras/file endpoint
</commit_message>
<xml_diff>
--- a/src/static/reports/InfoCarreras.xlsx
+++ b/src/static/reports/InfoCarreras.xlsx
@@ -450,13 +450,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -466,13 +466,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>